<commit_message>
updated files for submission
- added recording of code
</commit_message>
<xml_diff>
--- a/Homework/HW1/part b.xlsx
+++ b/Homework/HW1/part b.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eli/Documents/Code-Stuff/College/CSI 403/Homework/HW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DABC43-1283-754E-9EB1-2C0D939E454A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AC6DC9-381C-9548-A4E3-0279509A5679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="28200" windowHeight="16640" xr2:uid="{D57B2221-5B0D-AE4C-9FA8-67F896EA2AA7}"/>
+    <workbookView xWindow="13380" yWindow="0" windowWidth="15420" windowHeight="16700" xr2:uid="{D57B2221-5B0D-AE4C-9FA8-67F896EA2AA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,40 +138,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -300,10 +277,264 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
+              <a:round/>
+              <a:tailEnd type="stealth" w="lg" len="sm"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8286-5C4A-947D-6EAA9F6BA882}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time Used by Divide and Conquer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+              <a:headEnd type="none"/>
+              <a:tailEnd type="stealth" w="lg" len="sm"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8286-5C4A-947D-6EAA9F6BA882}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>f(n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="sq" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="9344D0">
+                  <a:alpha val="83000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+              <a:headEnd type="none"/>
+              <a:tailEnd type="none" w="lg" len="lg"/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.6666666666666664E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>666.66666666666663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8286-5C4A-947D-6EAA9F6BA882}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g(n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000">
+                  <a:alpha val="83000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -340,264 +571,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>664</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8286-5C4A-947D-6EAA9F6BA882}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time Used by Divide and Conquer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8286-5C4A-947D-6EAA9F6BA882}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>f(n)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="9344D0"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$3:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.6666666666666664E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.6666666666666666E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>666.66666666666663</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8286-5C4A-947D-6EAA9F6BA882}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g(n)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$E$3:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.8685845533741414</c:v>
+                  <c:v>4.1524101186092037E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7371691067482828</c:v>
+                  <c:v>8.3048202372184077E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6057536601224243</c:v>
+                  <c:v>1.2457230355827609</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4743382134965657</c:v>
+                  <c:v>16.609640474436812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,7 +1790,7 @@
   <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1811,7 +1799,8 @@
     <col min="3" max="3" width="28.1640625" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1824,16 +1813,16 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1847,21 +1836,21 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <f>F3*A3^2</f>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="E3" s="11">
-        <f xml:space="preserve"> G3 * LOG(A3,2)</f>
-        <v>1.8685845533741414</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="E3" s="8">
+        <f xml:space="preserve"> G3 * A3 * LOG(A3,2)</f>
+        <v>4.1524101186092037E-3</v>
+      </c>
+      <c r="F3" s="7">
         <f>1/150000</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="G3" s="12">
-        <f>9/16</f>
-        <v>0.5625</v>
+      <c r="G3" s="9">
+        <f>1/8000</f>
+        <v>1.25E-4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1874,13 +1863,13 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <f t="shared" ref="D4:D6" si="0">F4*A4^2</f>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" ref="E4:E6" si="1" xml:space="preserve"> G4 * LOG(A4,2)</f>
-        <v>3.7371691067482828</v>
+        <f t="shared" ref="E4:E6" si="1" xml:space="preserve"> G4 * A4 * LOG(A4,2)</f>
+        <v>8.3048202372184077E-2</v>
       </c>
       <c r="F4" s="1">
         <f>F3</f>
@@ -1888,7 +1877,7 @@
       </c>
       <c r="G4" s="1">
         <f>G3</f>
-        <v>0.5625</v>
+        <v>1.25E-4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1901,13 +1890,13 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
       <c r="E5" s="8">
         <f t="shared" si="1"/>
-        <v>5.6057536601224243</v>
+        <v>1.2457230355827609</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F6" si="2">F4</f>
@@ -1915,7 +1904,7 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" ref="G5:G6" si="3">G4</f>
-        <v>0.5625</v>
+        <v>1.25E-4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1928,13 +1917,13 @@
       <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>666.66666666666663</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="1"/>
-        <v>7.4743382134965657</v>
+        <v>16.609640474436812</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="2"/>
@@ -1942,18 +1931,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="3"/>
-        <v>0.5625</v>
+        <v>1.25E-4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>